<commit_message>
Modified the code so that pedigrees will be generated for each individual that will be a proband
Added accession_file.py which will generate accesion file
</commit_message>
<xml_diff>
--- a/_fam_sub_mot_fat_sam_sex_con_con_con_use_sra_twn.xlsx
+++ b/_fam_sub_mot_fat_sam_sex_con_con_con_use_sra_twn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinesong/Documents/2022/Park Lab/UGRP/venv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinesong/Documents/2022/Park Lab/cgap-pipeline-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B67F85A-38B6-F24D-B974-7E87951A1E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4770DFFD-31B2-5E4B-B1F4-ED0B421A7684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2233,8 +2233,8 @@
   <dimension ref="A1:N604"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A574" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J599" sqref="J599"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G588" activeCellId="4" sqref="G149:G188 G360:G395 G477:G493 G517:G533 G588:G603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>